<commit_message>
Update Mapping Property for current report with B3 Model
There are issue about how to get the league name , consider parentid ot
parentpartid. Event status to get status of event ot betting offer name
to get status return ?
</commit_message>
<xml_diff>
--- a/pushclient/documents/scores_odds history.xlsx
+++ b/pushclient/documents/scores_odds history.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ebbe\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hau Nguyen Thanh Nam\git\b3\pushclient\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28155" windowHeight="12030"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28152" windowHeight="12036"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="93">
   <si>
     <t>Time</t>
   </si>
@@ -187,12 +187,129 @@
   </si>
   <si>
     <t>Mark outliers in PEACH (as defined by a formula)</t>
+  </si>
+  <si>
+    <t>all filter can be found in betbrain model</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>B3 Table</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>SportId</t>
+  </si>
+  <si>
+    <t>Football</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Event.SportId</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>LocationId</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter </t>
+  </si>
+  <si>
+    <t>League</t>
+  </si>
+  <si>
+    <t>EventPart</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>EventPartId</t>
+  </si>
+  <si>
+    <t>English Permier League</t>
+  </si>
+  <si>
+    <t>Event.ParentEventPartId</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Event.Name, EventType = Match</t>
+  </si>
+  <si>
+    <t>Manu vs Arsenal</t>
+  </si>
+  <si>
+    <t>BettingType</t>
+  </si>
+  <si>
+    <t>BettingTypeId</t>
+  </si>
+  <si>
+    <t>EventId</t>
+  </si>
+  <si>
+    <t>BettingOffer.NettingTypeId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asian Handicap </t>
+  </si>
+  <si>
+    <t>OutcomeId</t>
+  </si>
+  <si>
+    <t>First Half</t>
+  </si>
+  <si>
+    <t>+1.5</t>
+  </si>
+  <si>
+    <t>BettingOffer.OutcomeId</t>
+  </si>
+  <si>
+    <t>BettingOffer.TimeStamp</t>
+  </si>
+  <si>
+    <t>Provider.popularity</t>
+  </si>
+  <si>
+    <t>Provider.Name</t>
+  </si>
+  <si>
+    <t>BettingOffer.Odds</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Event.VenueId</t>
+  </si>
+  <si>
+    <t>BettingOffer.Event.Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -250,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,6 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,23 +682,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S47"/>
+  <dimension ref="A2:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="C9" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="11"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="11"/>
+    <col min="2" max="2" width="24.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="18.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="17.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L2" s="5" t="s">
         <v>17</v>
       </c>
@@ -588,7 +711,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -605,7 +728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L4" s="2" t="s">
         <v>18</v>
       </c>
@@ -613,7 +736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>30</v>
       </c>
@@ -624,7 +747,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L6" s="2" t="s">
         <v>20</v>
       </c>
@@ -632,7 +755,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -646,7 +769,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>13</v>
       </c>
@@ -666,7 +789,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>0</v>
       </c>
@@ -698,7 +821,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>0.3972222222222222</v>
       </c>
@@ -730,7 +853,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>0.39756944444444442</v>
       </c>
@@ -762,7 +885,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L12" s="2" t="s">
         <v>25</v>
       </c>
@@ -770,7 +893,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="L13" s="2" t="s">
         <v>38</v>
       </c>
@@ -778,7 +901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -792,7 +915,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -806,7 +929,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
         <v>0</v>
       </c>
@@ -832,7 +955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="4">
         <v>0.3972222222222222</v>
       </c>
@@ -858,7 +981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="4">
         <v>0.39756944444444442</v>
       </c>
@@ -884,15 +1007,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="L21" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>13</v>
       </c>
@@ -905,8 +1031,23 @@
       <c r="E22" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>67</v>
+      </c>
+      <c r="K22" t="s">
+        <v>66</v>
+      </c>
+      <c r="L22" t="s">
+        <v>70</v>
+      </c>
+      <c r="N22" t="s">
+        <v>55</v>
+      </c>
+      <c r="P22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>0</v>
       </c>
@@ -931,8 +1072,23 @@
       <c r="I23" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="4">
         <v>0.3972222222222222</v>
       </c>
@@ -957,8 +1113,23 @@
       <c r="I24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K24" t="s">
+        <v>63</v>
+      </c>
+      <c r="L24" t="s">
+        <v>64</v>
+      </c>
+      <c r="N24" t="s">
+        <v>65</v>
+      </c>
+      <c r="P24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="4">
         <v>0.39756944444444442</v>
       </c>
@@ -983,76 +1154,261 @@
       <c r="I25" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>68</v>
+      </c>
+      <c r="K25" t="s">
+        <v>69</v>
+      </c>
+      <c r="L25" t="s">
+        <v>71</v>
+      </c>
+      <c r="N25" t="s">
+        <v>72</v>
+      </c>
+      <c r="P25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>61</v>
+      </c>
+      <c r="K26" t="s">
+        <v>61</v>
+      </c>
+      <c r="L26" t="s">
+        <v>79</v>
+      </c>
+      <c r="N26" t="s">
+        <v>76</v>
+      </c>
+      <c r="P26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>74</v>
+      </c>
+      <c r="K27" t="s">
+        <v>77</v>
+      </c>
+      <c r="L27" t="s">
+        <v>78</v>
+      </c>
+      <c r="N27" t="s">
+        <v>81</v>
+      </c>
+      <c r="P27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="J28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K28" t="s">
+        <v>29</v>
+      </c>
+      <c r="L28" t="s">
+        <v>82</v>
+      </c>
+      <c r="N28" t="s">
+        <v>83</v>
+      </c>
+      <c r="P28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>92</v>
+      </c>
+      <c r="I31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H32" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" t="s">
+        <v>92</v>
+      </c>
+      <c r="J32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="4"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="7" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C39" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="11">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="11">
         <v>2</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B42" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C42" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="11">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="11">
         <v>3</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B49" s="9" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1070,12 +1426,12 @@
       <selection activeCell="E5" sqref="E5:H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>26</v>
       </c>
@@ -1086,7 +1442,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>28</v>
       </c>

</xml_diff>